<commit_message>
Finializing the project with the needed out json files
</commit_message>
<xml_diff>
--- a/Seeds.xlsx
+++ b/Seeds.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Seeds for Brands Collection" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
   <si>
     <t>Test Case</t>
   </si>
@@ -79,9 +79,6 @@
     <t xml:space="preserve">Get the value of Array[0] and Insert Successfully </t>
   </si>
   <si>
-    <t>Field for TestCase</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -110,6 +107,20 @@
   </si>
   <si>
     <t xml:space="preserve">Write a default brand name and Insert Successfully </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix all typeos in both fields 
+and set the min value for both invalid field 
+and Insert Successfully </t>
+  </si>
+  <si>
+    <t>brandName,
+yearFounded , 
+numberOfLocations,
+headquarters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Violated Field(s) by TestCase</t>
   </si>
 </sst>
 </file>
@@ -197,17 +208,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H12" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:H12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H11" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H11"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Test Case" dataDxfId="7"/>
     <tableColumn id="2" name="_id" dataDxfId="6"/>
     <tableColumn id="3" name="brandName" dataDxfId="5"/>
     <tableColumn id="4" name="yearFounded" dataDxfId="4"/>
     <tableColumn id="5" name="numberOfLocations" dataDxfId="3"/>
-    <tableColumn id="7" name="headquarters" dataDxfId="1"/>
-    <tableColumn id="9" name="Use Case" dataDxfId="0"/>
-    <tableColumn id="6" name="Field for TestCase" dataDxfId="2"/>
+    <tableColumn id="7" name="headquarters" dataDxfId="2"/>
+    <tableColumn id="9" name="Use Case" dataDxfId="1"/>
+    <tableColumn id="6" name=" Violated Field(s) by TestCase" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -500,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +526,7 @@
     <col min="5" max="5" width="29.5703125" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="53.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -541,7 +552,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -567,7 +578,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -630,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -642,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>2</v>
@@ -685,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
@@ -694,7 +705,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>3</v>
@@ -714,13 +725,13 @@
         <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>4</v>
@@ -743,7 +754,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>16</v>
@@ -769,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>18</v>
@@ -778,51 +789,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>